<commit_message>
6-22 version finish, need create a branch for it. Then do rest task in 6-02 version.
</commit_message>
<xml_diff>
--- a/testExcel.xlsx
+++ b/testExcel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/young/workbench/code/python/future_trading/tqsdk/tqsdk_future_trading/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F3ECCEDB-2A0A-694B-9455-10298CD586CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{104D4147-E660-224A-8439-9ED97CA845D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11980" yWindow="5900" windowWidth="27640" windowHeight="16940" xr2:uid="{75AF422D-A1A3-D349-80FD-AB1A005C36E0}"/>
+    <workbookView xWindow="3420" yWindow="6120" windowWidth="36800" windowHeight="18160" xr2:uid="{1221F0E4-1EB9-2B47-B05C-E3CD8321B757}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="29">
   <si>
     <t>No</t>
   </si>
@@ -46,6 +46,9 @@
     <t>多空</t>
   </si>
   <si>
+    <t>买卖</t>
+  </si>
+  <si>
     <t>开仓时间</t>
   </si>
   <si>
@@ -67,19 +70,58 @@
     <t>手数</t>
   </si>
   <si>
-    <t>rb2210</t>
+    <t>SHFE.rb1805</t>
   </si>
   <si>
     <t>多</t>
   </si>
   <si>
-    <t>日线条件1</t>
-  </si>
-  <si>
-    <t>日线条件3</t>
-  </si>
-  <si>
-    <t>日线条件2</t>
+    <t>买</t>
+  </si>
+  <si>
+    <t>日线:3,2小时:2</t>
+  </si>
+  <si>
+    <t>卖</t>
+  </si>
+  <si>
+    <t>止损平仓,止损价3751.44</t>
+  </si>
+  <si>
+    <t>止损平仓,止损价3750.46</t>
+  </si>
+  <si>
+    <t>日线:2,2小时:1</t>
+  </si>
+  <si>
+    <t>止损平仓,止损价3837.68</t>
+  </si>
+  <si>
+    <t>SHFE.rb1810</t>
+  </si>
+  <si>
+    <t>日线:1,2小时:1</t>
+  </si>
+  <si>
+    <t>止盈条件:其他,盈亏比达到1:2,售出50%仓位</t>
+  </si>
+  <si>
+    <t>止损平仓,止损价3573.0</t>
+  </si>
+  <si>
+    <t>止损平仓,止损价3609.34</t>
+  </si>
+  <si>
+    <t>日线:2,2小时:2</t>
+  </si>
+  <si>
+    <t>换月平仓</t>
+  </si>
+  <si>
+    <t>SHFE.rb1901</t>
+  </si>
+  <si>
+    <t>止损平仓,止损价4081.7</t>
   </si>
 </sst>
 </file>
@@ -431,14 +473,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F26CF5D-3609-5747-A2BD-36A5F776C393}">
-  <dimension ref="A1:J4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F5E9466-6ABC-7B45-8DEB-BEEF70144CFB}">
+  <dimension ref="A1:K17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15:XFD15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="5" max="5" width="18.5" customWidth="1"/>
+    <col min="7" max="7" width="15.83203125" customWidth="1"/>
+    <col min="8" max="8" width="23.1640625" customWidth="1"/>
+    <col min="10" max="10" width="44.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -469,74 +519,424 @@
       <c r="J1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="1">
+        <v>43102.396516203706</v>
+      </c>
+      <c r="F2">
+        <v>3828</v>
+      </c>
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="1">
-        <v>44611.939386574071</v>
-      </c>
-      <c r="E2">
-        <v>4567</v>
-      </c>
-      <c r="F2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J2">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
       <c r="C3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="1">
-        <v>44611.939386574071</v>
-      </c>
-      <c r="E3">
-        <v>4567</v>
-      </c>
-      <c r="F3" t="s">
-        <v>13</v>
-      </c>
-      <c r="J3">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="1">
+        <v>43108.582627314812</v>
+      </c>
+      <c r="I3">
+        <v>3748</v>
+      </c>
+      <c r="J3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K3">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="1">
+        <v>43108.897210648145</v>
+      </c>
+      <c r="F4">
+        <v>3827</v>
+      </c>
+      <c r="G4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K4">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" s="1">
+        <v>43115.375</v>
+      </c>
+      <c r="I5">
+        <v>3750</v>
+      </c>
+      <c r="J5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K5">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="1">
+        <v>43124.379155092596</v>
+      </c>
+      <c r="F6">
+        <v>3916</v>
+      </c>
+      <c r="G6" t="s">
+        <v>18</v>
+      </c>
+      <c r="K6">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7" s="1">
+        <v>43167.566655092596</v>
+      </c>
+      <c r="I7">
+        <v>3834</v>
+      </c>
+      <c r="J7" t="s">
+        <v>19</v>
+      </c>
+      <c r="K7">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="1">
+        <v>43216.918738425928</v>
+      </c>
+      <c r="F8">
+        <v>3573</v>
+      </c>
+      <c r="G8" t="s">
+        <v>21</v>
+      </c>
+      <c r="K8">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H9" s="1">
+        <v>43222.613888888889</v>
+      </c>
+      <c r="I9">
+        <v>3716</v>
+      </c>
+      <c r="J9" t="s">
+        <v>22</v>
+      </c>
+      <c r="K9">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>7</v>
+      </c>
+      <c r="B10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" t="s">
+        <v>15</v>
+      </c>
+      <c r="H10" s="1">
+        <v>43229.59443287037</v>
+      </c>
+      <c r="I10">
+        <v>3573</v>
+      </c>
+      <c r="J10" t="s">
+        <v>23</v>
+      </c>
+      <c r="K10">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11">
         <v>10</v>
       </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="1">
-        <v>44611.939386574071</v>
-      </c>
-      <c r="E4">
-        <v>4567</v>
-      </c>
-      <c r="F4" t="s">
-        <v>14</v>
-      </c>
-      <c r="J4">
+      <c r="B11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" s="1">
+        <v>43235.93818287037</v>
+      </c>
+      <c r="F11">
+        <v>3683</v>
+      </c>
+      <c r="G11" t="s">
+        <v>18</v>
+      </c>
+      <c r="K11">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" t="s">
+        <v>15</v>
+      </c>
+      <c r="H12" s="1">
+        <v>43238.885405092595</v>
+      </c>
+      <c r="I12">
+        <v>3609</v>
+      </c>
+      <c r="J12" t="s">
+        <v>24</v>
+      </c>
+      <c r="K12">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="1">
+        <v>43244.875</v>
+      </c>
+      <c r="F13">
+        <v>3581</v>
+      </c>
+      <c r="G13" t="s">
+        <v>25</v>
+      </c>
+      <c r="K13">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" t="s">
+        <v>15</v>
+      </c>
+      <c r="H14" s="1">
+        <v>43251.890972222223</v>
+      </c>
+      <c r="I14">
+        <v>3721</v>
+      </c>
+      <c r="J14" t="s">
+        <v>22</v>
+      </c>
+      <c r="K14">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>12</v>
+      </c>
+      <c r="B15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" t="s">
+        <v>15</v>
+      </c>
+      <c r="H15" s="1">
+        <v>43361.624988425923</v>
+      </c>
+      <c r="I15">
+        <v>4184</v>
+      </c>
+      <c r="J15" t="s">
         <v>26</v>
+      </c>
+      <c r="K15">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" s="1">
+        <v>43395.611793981479</v>
+      </c>
+      <c r="F16">
+        <v>4165</v>
+      </c>
+      <c r="G16" t="s">
+        <v>18</v>
+      </c>
+      <c r="K16">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17" t="s">
+        <v>15</v>
+      </c>
+      <c r="H17" s="1">
+        <v>43405.572905092595</v>
+      </c>
+      <c r="I17">
+        <v>4077</v>
+      </c>
+      <c r="J17" t="s">
+        <v>28</v>
+      </c>
+      <c r="K17">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>